<commit_message>
Updating to the newest calculation engine, updating readme.
</commit_message>
<xml_diff>
--- a/PresentValueSeries/Cashflows.xlsx
+++ b/PresentValueSeries/Cashflows.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919EBAC4-7E3B-42AB-978B-302FDB192C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A0C50B-E8EC-40E2-82CA-F50AD6096C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="13460" windowHeight="6570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -1125,7 +1125,7 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="AmountType" dataDxfId="63"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="AocType" dataDxfId="62"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Novelty" dataDxfId="61"/>
-    <tableColumn id="67" xr3:uid="{732C3606-B4B3-405A-B2E0-0E4CBAB208AF}" name="AccidentYear"/>
+    <tableColumn id="66" xr3:uid="{36B38A32-6C1D-42BE-96D6-BCE9CFDE1C22}" name="AccidentYear"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Values0" dataDxfId="60"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Values1" dataDxfId="59"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Values2" dataDxfId="58"/>

</xml_diff>